<commit_message>
deleted:    inputs/Project1.xlsx 	deleted:    inputs/Project2.xlsx 	deleted:    inputs/Project3.xlsx 	modified:   src/config.ini 	modified:   src/utils.py
</commit_message>
<xml_diff>
--- a/inputs/Portfolio.xlsx
+++ b/inputs/Portfolio.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc_\Dropbox\MLosPython\PortfolioAlgorithm\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8E20B2-1E9E-499B-BE52-5EECE013DB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73673DE-06ED-4C13-BA91-EBCCE4362FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Project1" sheetId="1" r:id="rId1"/>
-    <sheet name="Project2" sheetId="3" r:id="rId2"/>
-    <sheet name="Project3" sheetId="4" r:id="rId3"/>
+    <sheet name="P1" sheetId="1" r:id="rId1"/>
+    <sheet name="P2" sheetId="3" r:id="rId2"/>
+    <sheet name="P3" sheetId="4" r:id="rId3"/>
     <sheet name="Resources" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -1550,7 +1550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+    <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -4612,8 +4612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFF8FDB7-9246-43A8-92D6-1A279CB8F8FD}">
   <dimension ref="A1:S988"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
bug fixing: generation of absolute dates
</commit_message>
<xml_diff>
--- a/inputs/Portfolio.xlsx
+++ b/inputs/Portfolio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc_\Dropbox\MLosPython\PortfolioAlgorithm\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032CBD0C-F30B-4CFC-966C-3257A04B34E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA9B331-C1C4-479A-9011-3CD61969EED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1" sheetId="1" r:id="rId1"/>
@@ -825,7 +825,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -924,6 +924,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="30">
@@ -1130,7 +1138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1264,6 +1272,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1547,8 +1556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3401,7 +3410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A37262CE-87B7-4331-90C8-185C1B22225A}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
@@ -6922,10 +6931,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D4820D-14BB-AB40-8F7C-C9AAA53F16A3}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6935,7 +6944,7 @@
     <col min="4" max="4" width="19.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>95</v>
       </c>
@@ -6949,7 +6958,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
         <v>102</v>
       </c>
@@ -6963,7 +6972,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
         <v>103</v>
       </c>
@@ -6977,7 +6986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
         <v>105</v>
       </c>
@@ -6991,7 +7000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
         <v>107</v>
       </c>
@@ -7005,7 +7014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="26" t="s">
         <v>108</v>
       </c>
@@ -7019,7 +7028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="26" t="s">
         <v>109</v>
       </c>
@@ -7033,7 +7042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="26" t="s">
         <v>110</v>
       </c>
@@ -7047,7 +7056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="26" t="s">
         <v>111</v>
       </c>
@@ -7060,8 +7069,9 @@
       <c r="D9" s="27">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9" s="55"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
         <v>112</v>
       </c>
@@ -7075,7 +7085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="26" t="s">
         <v>113</v>
       </c>
@@ -7089,7 +7099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
         <v>114</v>
       </c>
@@ -7103,7 +7113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="26" t="s">
         <v>115</v>
       </c>
@@ -7116,6 +7126,9 @@
       <c r="D13" s="27">
         <v>2</v>
       </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D14" s="55"/>
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>

</xml_diff>

<commit_message>
Major update to combine projects before algorithm
</commit_message>
<xml_diff>
--- a/inputs/Portfolio.xlsx
+++ b/inputs/Portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marc_\Dropbox\MLosPython\PortfolioAlgorithm\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE434B7-E93F-44E5-AB1B-0A6F4F989D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCCF16B-9CAF-4912-97BD-7937468C4123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -317,511 +317,511 @@
     <t xml:space="preserve">   Contracts closure</t>
   </si>
   <si>
+    <t xml:space="preserve">   Project closing report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ACCEPTANCE Project 1</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Predecessors</t>
+  </si>
+  <si>
+    <t>Successors</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Sanitary water system</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>Pipeline system</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>Architect Sr</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>Architect Jr</t>
+  </si>
+  <si>
+    <t>Engineer Sr</t>
+  </si>
+  <si>
+    <t>Engineer Jr</t>
+  </si>
+  <si>
+    <t>PM 1</t>
+  </si>
+  <si>
+    <t>PM 2</t>
+  </si>
+  <si>
+    <t>PM 3</t>
+  </si>
+  <si>
+    <t>Quality Manager Sr</t>
+  </si>
+  <si>
+    <t>Quality Manager Jr</t>
+  </si>
+  <si>
+    <t>Lawyer and Legal Specialist</t>
+  </si>
+  <si>
+    <t>Procurement Manager</t>
+  </si>
+  <si>
+    <t>Procurement Assistant</t>
+  </si>
+  <si>
+    <t>25FC+5</t>
+  </si>
+  <si>
+    <t>32FC+8</t>
+  </si>
+  <si>
+    <t>37FC+5</t>
+  </si>
+  <si>
+    <t>42FC+5</t>
+  </si>
+  <si>
+    <t>48FC+5</t>
+  </si>
+  <si>
+    <t>49FC+2</t>
+  </si>
+  <si>
+    <t>26FC+5</t>
+  </si>
+  <si>
+    <t>34;35;36FC+8</t>
+  </si>
+  <si>
+    <t>38FC+5</t>
+  </si>
+  <si>
+    <t>43;45FC+5;47</t>
+  </si>
+  <si>
+    <t>49FC+5</t>
+  </si>
+  <si>
+    <t>50;51;52FC+2</t>
+  </si>
+  <si>
+    <t>Electrical system</t>
+  </si>
+  <si>
+    <t>Pred other projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Contract signing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Project planning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Project execution and controlling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Documentation analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Consultation results report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Architectural design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Lanscape design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Final design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Legal permits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Environmental permits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Construction license</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Providers contracts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Components contracts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Procurement documents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Site preparation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Sanitary Water system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Electrical system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Soccer field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Changing rooms &amp; toilettes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Gym</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Leisure area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Garden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Roads</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Decorative elements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Lagoon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Urban metallic components installment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Soccer field and leisure zone components installment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Installation of water dispensers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Equipment functionality test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Final test supporting document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Operations manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Contracts closure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Project closing report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      ACCEPTANCE Project 1</t>
+  </si>
+  <si>
+    <t>Contract signing</t>
+  </si>
+  <si>
+    <t>Project planning</t>
+  </si>
+  <si>
+    <t>Project execution and controlling</t>
+  </si>
+  <si>
+    <t>Area survey</t>
+  </si>
+  <si>
+    <t>Topographic study</t>
+  </si>
+  <si>
+    <t>Conceptual design</t>
+  </si>
+  <si>
+    <t>Architectural design</t>
+  </si>
+  <si>
+    <t>Bidding</t>
+  </si>
+  <si>
+    <t>Equipment contracts</t>
+  </si>
+  <si>
+    <t>Legal permits</t>
+  </si>
+  <si>
+    <t>Construction license</t>
+  </si>
+  <si>
+    <t>Operations licenses</t>
+  </si>
+  <si>
+    <t>Existing structure demolition</t>
+  </si>
+  <si>
+    <t>Debris removal</t>
+  </si>
+  <si>
+    <t>Earthmoving works</t>
+  </si>
+  <si>
+    <t>Foundations</t>
+  </si>
+  <si>
+    <t>Reinforced concrete structure</t>
+  </si>
+  <si>
+    <t>Vertical walls</t>
+  </si>
+  <si>
+    <t>Thermo-acoustic insulation</t>
+  </si>
+  <si>
+    <t>Walls plaster</t>
+  </si>
+  <si>
+    <t>Mechanical system</t>
+  </si>
+  <si>
+    <t>Floor covering</t>
+  </si>
+  <si>
+    <t>Windows and doors placement</t>
+  </si>
+  <si>
+    <t>Wall patching</t>
+  </si>
+  <si>
+    <t>Painting walls</t>
+  </si>
+  <si>
+    <t>Electrical appliances installment</t>
+  </si>
+  <si>
+    <t>Sanitary facilities installment</t>
+  </si>
+  <si>
+    <t>Furnitures</t>
+  </si>
+  <si>
+    <t>Equipment functionality test</t>
+  </si>
+  <si>
+    <t>Equipment installment acceptance</t>
+  </si>
+  <si>
+    <t>Building site final cleaning</t>
+  </si>
+  <si>
+    <t>Final test supporting document</t>
+  </si>
+  <si>
+    <t>Operations manual</t>
+  </si>
+  <si>
+    <t>Contracts closure</t>
+  </si>
+  <si>
+    <t>Project closing report</t>
+  </si>
+  <si>
+    <t>ACCEPTANCE Project 1</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>7;8</t>
+  </si>
+  <si>
+    <t>17;18;19;20;21;22;23;24;25;26</t>
+  </si>
+  <si>
+    <t>27;28;29</t>
+  </si>
+  <si>
+    <t>16;17;18;19;20;21;22;23;24;25;26;27;28;29</t>
+  </si>
+  <si>
+    <t>10;11;12;15</t>
+  </si>
+  <si>
+    <t>13;15;16</t>
+  </si>
+  <si>
+    <t>13;15;17</t>
+  </si>
+  <si>
+    <t>19;20</t>
+  </si>
+  <si>
+    <t>13;15;18</t>
+  </si>
+  <si>
+    <t>13;15;18;19</t>
+  </si>
+  <si>
+    <t>13;15;20</t>
+  </si>
+  <si>
+    <t>13;15;21</t>
+  </si>
+  <si>
+    <t>13;15;22</t>
+  </si>
+  <si>
+    <t>24;27</t>
+  </si>
+  <si>
+    <t>13;15;23</t>
+  </si>
+  <si>
+    <t>25;26;27</t>
+  </si>
+  <si>
+    <t>13;15;24</t>
+  </si>
+  <si>
+    <t>14;15;23;24;25;26</t>
+  </si>
+  <si>
+    <t>14;15;27</t>
+  </si>
+  <si>
+    <t>14;15;28</t>
+  </si>
+  <si>
+    <t>6FC+5</t>
+  </si>
+  <si>
+    <t>9FC+20</t>
+  </si>
+  <si>
+    <t>9FC+35</t>
+  </si>
+  <si>
+    <t>7;8FC+5</t>
+  </si>
+  <si>
+    <t>10;11;12;13FC+20;14FC+35;15</t>
+  </si>
+  <si>
+    <t>7;5</t>
+  </si>
+  <si>
+    <t>9;13</t>
+  </si>
+  <si>
+    <t>14;26;22;10</t>
+  </si>
+  <si>
+    <t>30;31;32;11</t>
+  </si>
+  <si>
+    <t>14;12</t>
+  </si>
+  <si>
+    <t>11;12;9</t>
+  </si>
+  <si>
+    <t>9;21</t>
+  </si>
+  <si>
+    <t>25;30</t>
+  </si>
+  <si>
+    <t>26;30</t>
+  </si>
+  <si>
+    <t>9;25</t>
+  </si>
+  <si>
+    <t>10;29;25;24</t>
+  </si>
+  <si>
+    <t>30;10;29</t>
+  </si>
+  <si>
+    <t>32;33</t>
+  </si>
+  <si>
+    <t>31;10</t>
+  </si>
+  <si>
+    <t>34;33</t>
+  </si>
+  <si>
+    <t>31;32</t>
+  </si>
+  <si>
+    <t>33;32</t>
+  </si>
+  <si>
+    <t>13;35</t>
+  </si>
+  <si>
+    <t>6FC+5;8</t>
+  </si>
+  <si>
+    <t>5FC+5</t>
+  </si>
+  <si>
+    <t>32;4</t>
+  </si>
+  <si>
+    <t>37;4</t>
+  </si>
+  <si>
     <t>4;55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Project closing report</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   ACCEPTANCE Project 1</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Section</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Duration</t>
-  </si>
-  <si>
-    <t>Predecessors</t>
-  </si>
-  <si>
-    <t>Successors</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>Sanitary water system</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>Pipeline system</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>Architect Sr</t>
-  </si>
-  <si>
-    <t>HC</t>
-  </si>
-  <si>
-    <t>Architect Jr</t>
-  </si>
-  <si>
-    <t>Engineer Sr</t>
-  </si>
-  <si>
-    <t>Engineer Jr</t>
-  </si>
-  <si>
-    <t>PM 1</t>
-  </si>
-  <si>
-    <t>PM 2</t>
-  </si>
-  <si>
-    <t>PM 3</t>
-  </si>
-  <si>
-    <t>Quality Manager Sr</t>
-  </si>
-  <si>
-    <t>Quality Manager Jr</t>
-  </si>
-  <si>
-    <t>Lawyer and Legal Specialist</t>
-  </si>
-  <si>
-    <t>Procurement Manager</t>
-  </si>
-  <si>
-    <t>Procurement Assistant</t>
-  </si>
-  <si>
-    <t>25FC+5</t>
-  </si>
-  <si>
-    <t>32FC+8</t>
-  </si>
-  <si>
-    <t>37FC+5</t>
-  </si>
-  <si>
-    <t>42FC+5</t>
-  </si>
-  <si>
-    <t>48FC+5</t>
-  </si>
-  <si>
-    <t>49FC+2</t>
-  </si>
-  <si>
-    <t>26FC+5</t>
-  </si>
-  <si>
-    <t>34;35;36FC+8</t>
-  </si>
-  <si>
-    <t>38FC+5</t>
-  </si>
-  <si>
-    <t>43;45FC+5;47</t>
-  </si>
-  <si>
-    <t>49FC+5</t>
-  </si>
-  <si>
-    <t>50;51;52FC+2</t>
-  </si>
-  <si>
-    <t>Electrical system</t>
-  </si>
-  <si>
-    <t>Pred other projects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Contract signing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Project planning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Project execution and controlling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Documentation analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Consultation results report</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Architectural design</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Lanscape design</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Final design</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Legal permits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Environmental permits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Construction license</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Providers contracts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Components contracts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Procurement documents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Site preparation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Sanitary Water system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Electrical system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Soccer field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Changing rooms &amp; toilettes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Gym</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Leisure area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Garden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Roads</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Decorative elements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Lagoon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Urban metallic components installment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Soccer field and leisure zone components installment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Installation of water dispensers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Equipment functionality test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Final test supporting document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Operations manual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Contracts closure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      Project closing report</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ACCEPTANCE Project 1</t>
-  </si>
-  <si>
-    <t>Contract signing</t>
-  </si>
-  <si>
-    <t>Project planning</t>
-  </si>
-  <si>
-    <t>Project execution and controlling</t>
-  </si>
-  <si>
-    <t>Area survey</t>
-  </si>
-  <si>
-    <t>Topographic study</t>
-  </si>
-  <si>
-    <t>Conceptual design</t>
-  </si>
-  <si>
-    <t>Architectural design</t>
-  </si>
-  <si>
-    <t>Bidding</t>
-  </si>
-  <si>
-    <t>Equipment contracts</t>
-  </si>
-  <si>
-    <t>Legal permits</t>
-  </si>
-  <si>
-    <t>Construction license</t>
-  </si>
-  <si>
-    <t>Operations licenses</t>
-  </si>
-  <si>
-    <t>Existing structure demolition</t>
-  </si>
-  <si>
-    <t>Debris removal</t>
-  </si>
-  <si>
-    <t>Earthmoving works</t>
-  </si>
-  <si>
-    <t>Foundations</t>
-  </si>
-  <si>
-    <t>Reinforced concrete structure</t>
-  </si>
-  <si>
-    <t>Vertical walls</t>
-  </si>
-  <si>
-    <t>Thermo-acoustic insulation</t>
-  </si>
-  <si>
-    <t>Walls plaster</t>
-  </si>
-  <si>
-    <t>Mechanical system</t>
-  </si>
-  <si>
-    <t>Floor covering</t>
-  </si>
-  <si>
-    <t>Windows and doors placement</t>
-  </si>
-  <si>
-    <t>Wall patching</t>
-  </si>
-  <si>
-    <t>Painting walls</t>
-  </si>
-  <si>
-    <t>Electrical appliances installment</t>
-  </si>
-  <si>
-    <t>Sanitary facilities installment</t>
-  </si>
-  <si>
-    <t>Furnitures</t>
-  </si>
-  <si>
-    <t>Equipment functionality test</t>
-  </si>
-  <si>
-    <t>Equipment installment acceptance</t>
-  </si>
-  <si>
-    <t>Building site final cleaning</t>
-  </si>
-  <si>
-    <t>Final test supporting document</t>
-  </si>
-  <si>
-    <t>Operations manual</t>
-  </si>
-  <si>
-    <t>Contracts closure</t>
-  </si>
-  <si>
-    <t>Project closing report</t>
-  </si>
-  <si>
-    <t>ACCEPTANCE Project 1</t>
-  </si>
-  <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>7;8</t>
-  </si>
-  <si>
-    <t>17;18;19;20;21;22;23;24;25;26</t>
-  </si>
-  <si>
-    <t>27;28;29</t>
-  </si>
-  <si>
-    <t>16;17;18;19;20;21;22;23;24;25;26;27;28;29</t>
-  </si>
-  <si>
-    <t>10;11;12;15</t>
-  </si>
-  <si>
-    <t>13;15;16</t>
-  </si>
-  <si>
-    <t>13;15;17</t>
-  </si>
-  <si>
-    <t>19;20</t>
-  </si>
-  <si>
-    <t>13;15;18</t>
-  </si>
-  <si>
-    <t>13;15;18;19</t>
-  </si>
-  <si>
-    <t>13;15;20</t>
-  </si>
-  <si>
-    <t>13;15;21</t>
-  </si>
-  <si>
-    <t>13;15;22</t>
-  </si>
-  <si>
-    <t>24;27</t>
-  </si>
-  <si>
-    <t>13;15;23</t>
-  </si>
-  <si>
-    <t>25;26;27</t>
-  </si>
-  <si>
-    <t>13;15;24</t>
-  </si>
-  <si>
-    <t>14;15;23;24;25;26</t>
-  </si>
-  <si>
-    <t>14;15;27</t>
-  </si>
-  <si>
-    <t>14;15;28</t>
-  </si>
-  <si>
-    <t>6FC+5</t>
-  </si>
-  <si>
-    <t>9FC+20</t>
-  </si>
-  <si>
-    <t>9FC+35</t>
-  </si>
-  <si>
-    <t>7;8FC+5</t>
-  </si>
-  <si>
-    <t>10;11;12;13FC+20;14FC+35;15</t>
-  </si>
-  <si>
-    <t>7;5</t>
-  </si>
-  <si>
-    <t>9;13</t>
-  </si>
-  <si>
-    <t>14;26;22;10</t>
-  </si>
-  <si>
-    <t>30;31;32;11</t>
-  </si>
-  <si>
-    <t>14;12</t>
-  </si>
-  <si>
-    <t>11;12;9</t>
-  </si>
-  <si>
-    <t>9;21</t>
-  </si>
-  <si>
-    <t>25;30</t>
-  </si>
-  <si>
-    <t>26;30</t>
-  </si>
-  <si>
-    <t>9;25</t>
-  </si>
-  <si>
-    <t>10;29;25;24</t>
-  </si>
-  <si>
-    <t>30;10;29</t>
-  </si>
-  <si>
-    <t>32;33</t>
-  </si>
-  <si>
-    <t>31;10</t>
-  </si>
-  <si>
-    <t>34;33</t>
-  </si>
-  <si>
-    <t>31;32</t>
-  </si>
-  <si>
-    <t>33;32</t>
-  </si>
-  <si>
-    <t>13;35</t>
-  </si>
-  <si>
-    <t>6FC+5;8</t>
-  </si>
-  <si>
-    <t>5FC+5</t>
-  </si>
-  <si>
-    <t>32;4</t>
-  </si>
-  <si>
-    <t>37;4</t>
   </si>
 </sst>
 </file>
@@ -1560,7 +1560,7 @@
   <dimension ref="A1:S58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1577,61 +1577,61 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="24" t="s">
-        <v>100</v>
-      </c>
       <c r="G1" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H1" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="I1" s="24" t="s">
-        <v>103</v>
-      </c>
       <c r="J1" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K1" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="N1" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="O1" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="P1" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="Q1" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="R1" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="S1" s="24" t="s">
         <v>114</v>
-      </c>
-      <c r="S1" s="24" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.35">
@@ -2372,7 +2372,7 @@
         <v>41</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G25" s="22"/>
       <c r="H25" s="28"/>
@@ -2399,7 +2399,7 @@
         <v>5</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F26" s="22" t="s">
         <v>43</v>
@@ -2582,7 +2582,7 @@
         <v>55</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G32" s="17"/>
       <c r="H32" s="28"/>
@@ -2699,7 +2699,7 @@
         <v>3</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F36" s="17">
         <v>37</v>
@@ -2732,7 +2732,7 @@
         <v>62</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G37" s="17"/>
       <c r="H37" s="28"/>
@@ -2759,7 +2759,7 @@
         <v>5</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F38" s="17" t="s">
         <v>64</v>
@@ -2882,7 +2882,7 @@
         <v>72</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G42" s="19"/>
       <c r="H42" s="28"/>
@@ -2969,7 +2969,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F45" s="19">
         <v>48</v>
@@ -3062,7 +3062,7 @@
         <v>81</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G48" s="19"/>
       <c r="H48" s="28"/>
@@ -3089,10 +3089,10 @@
         <v>5</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G49" s="19"/>
       <c r="H49" s="28"/>
@@ -3179,7 +3179,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F52" s="19">
         <v>53</v>
@@ -3317,7 +3317,7 @@
         <v>3</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>92</v>
+        <v>260</v>
       </c>
       <c r="F56" s="21">
         <v>57</v>
@@ -3349,7 +3349,7 @@
         <v>57</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D57" s="2">
         <v>1</v>
@@ -3381,7 +3381,7 @@
         <v>58</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D58" s="2">
         <v>0</v>
@@ -3432,61 +3432,61 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="24" t="s">
-        <v>100</v>
-      </c>
       <c r="G1" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H1" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="I1" s="24" t="s">
-        <v>103</v>
-      </c>
       <c r="J1" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K1" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="N1" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="O1" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="P1" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="Q1" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="R1" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="S1" s="24" t="s">
         <v>114</v>
-      </c>
-      <c r="S1" s="24" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.35">
@@ -3494,7 +3494,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -3522,7 +3522,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D3" s="2">
         <v>60</v>
@@ -3554,7 +3554,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D4" s="2">
         <v>500</v>
@@ -3586,7 +3586,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D5" s="2">
         <v>30</v>
@@ -3620,7 +3620,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D6" s="2">
         <v>30</v>
@@ -3629,7 +3629,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="28">
@@ -3658,7 +3658,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D7" s="2">
         <v>20</v>
@@ -3692,13 +3692,13 @@
         <v>8</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D8" s="2">
         <v>15</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F8" s="13">
         <v>9</v>
@@ -3726,16 +3726,16 @@
         <v>9</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D9" s="2">
         <v>20</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="28">
@@ -3764,7 +3764,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D10" s="2">
         <v>30</v>
@@ -3796,7 +3796,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D11" s="2">
         <v>30</v>
@@ -3828,7 +3828,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D12" s="2">
         <v>30</v>
@@ -3860,16 +3860,16 @@
         <v>13</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D13" s="2">
         <v>45</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="28"/>
@@ -3894,16 +3894,16 @@
         <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D14" s="2">
         <v>30</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="28"/>
@@ -3928,7 +3928,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D15" s="2">
         <v>70</v>
@@ -3937,7 +3937,7 @@
         <v>9</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="28"/>
@@ -3962,13 +3962,13 @@
         <v>16</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D16" s="2">
         <v>25</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F16" s="13">
         <v>17</v>
@@ -3992,13 +3992,13 @@
         <v>17</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D17" s="2">
         <v>18</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F17" s="13">
         <v>18</v>
@@ -4022,16 +4022,16 @@
         <v>18</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D18" s="2">
         <v>43</v>
       </c>
       <c r="E18" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="F18" s="13" t="s">
         <v>220</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>221</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="28"/>
@@ -4052,13 +4052,13 @@
         <v>19</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D19" s="2">
         <v>36</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F19" s="13">
         <v>20</v>
@@ -4082,13 +4082,13 @@
         <v>20</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D20" s="2">
         <v>39</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F20" s="13">
         <v>21</v>
@@ -4112,13 +4112,13 @@
         <v>21</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D21" s="2">
         <v>15</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F21" s="13">
         <v>22</v>
@@ -4142,13 +4142,13 @@
         <v>22</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D22" s="2">
         <v>7</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F22" s="13">
         <v>23</v>
@@ -4172,16 +4172,16 @@
         <v>23</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D23" s="2">
         <v>10</v>
       </c>
       <c r="E23" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="F23" s="13" t="s">
         <v>226</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>227</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="28"/>
@@ -4202,16 +4202,16 @@
         <v>24</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D24" s="2">
         <v>10</v>
       </c>
       <c r="E24" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="F24" s="13" t="s">
         <v>228</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>229</v>
       </c>
       <c r="G24" s="13"/>
       <c r="H24" s="28"/>
@@ -4232,13 +4232,13 @@
         <v>25</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D25" s="2">
         <v>5</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F25" s="13">
         <v>27</v>
@@ -4262,13 +4262,13 @@
         <v>26</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D26" s="2">
         <v>60</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F26" s="13">
         <v>27</v>
@@ -4292,13 +4292,13 @@
         <v>27</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D27" s="2">
         <v>22</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F27" s="13">
         <v>28</v>
@@ -4322,13 +4322,13 @@
         <v>28</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D28" s="2">
         <v>15</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F28" s="13">
         <v>29</v>
@@ -4352,13 +4352,13 @@
         <v>29</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D29" s="2">
         <v>15</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F29" s="13">
         <v>30</v>
@@ -4382,7 +4382,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D30" s="2">
         <v>15</v>
@@ -4424,7 +4424,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D31" s="2">
         <v>10</v>
@@ -4462,7 +4462,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D32" s="2">
         <v>5</v>
@@ -4500,13 +4500,13 @@
         <v>33</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D33" s="2">
         <v>3</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F33" s="13">
         <v>34</v>
@@ -4538,7 +4538,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D34" s="2">
         <v>1</v>
@@ -4570,7 +4570,7 @@
         <v>35</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
@@ -4639,61 +4639,61 @@
   <sheetData>
     <row r="1" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="C1" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="E1" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="F1" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="38" t="s">
-        <v>100</v>
-      </c>
       <c r="G1" s="38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H1" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="I1" s="24" t="s">
-        <v>103</v>
-      </c>
       <c r="J1" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K1" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="M1" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="N1" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="O1" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="P1" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="Q1" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="R1" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="S1" s="24" t="s">
         <v>114</v>
-      </c>
-      <c r="S1" s="24" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.35">
@@ -4701,7 +4701,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D2" s="41">
         <v>0</v>
@@ -4729,7 +4729,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D3" s="41">
         <v>40</v>
@@ -4761,7 +4761,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D4" s="41">
         <v>850</v>
@@ -4793,7 +4793,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D5" s="41">
         <v>15</v>
@@ -4802,7 +4802,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="43" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G5" s="43"/>
       <c r="H5" s="44">
@@ -4831,13 +4831,13 @@
         <v>6</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D6" s="41">
         <v>8</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F6" s="43">
         <v>7</v>
@@ -4865,7 +4865,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D7" s="41">
         <v>8</v>
@@ -4903,16 +4903,16 @@
         <v>8</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D8" s="41">
         <v>15</v>
       </c>
       <c r="E8" s="43" t="s">
+        <v>238</v>
+      </c>
+      <c r="F8" s="43" t="s">
         <v>239</v>
-      </c>
-      <c r="F8" s="43" t="s">
-        <v>240</v>
       </c>
       <c r="G8" s="43"/>
       <c r="H8" s="44">
@@ -4941,7 +4941,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D9" s="41">
         <v>32</v>
@@ -4950,7 +4950,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="43" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G9" s="43"/>
       <c r="H9" s="44">
@@ -4983,7 +4983,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D10" s="41">
         <v>14</v>
@@ -4992,7 +4992,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="43" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G10" s="43"/>
       <c r="H10" s="44">
@@ -5025,7 +5025,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D11" s="41">
         <v>15</v>
@@ -5034,7 +5034,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G11" s="43"/>
       <c r="H11" s="44"/>
@@ -5057,7 +5057,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D12" s="41">
         <v>15</v>
@@ -5093,7 +5093,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D13" s="41">
         <v>15</v>
@@ -5129,13 +5129,13 @@
         <v>14</v>
       </c>
       <c r="C14" s="49" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D14" s="41">
         <v>10</v>
       </c>
       <c r="E14" s="43" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F14" s="43">
         <v>15</v>
@@ -5159,7 +5159,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="49" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D15" s="41">
         <v>10</v>
@@ -5189,7 +5189,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D16" s="41">
         <v>15</v>
@@ -5219,7 +5219,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D17" s="41">
         <v>15</v>
@@ -5249,7 +5249,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="49" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D18" s="41">
         <v>15</v>
@@ -5279,7 +5279,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D19" s="41">
         <v>60</v>
@@ -5309,7 +5309,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D20" s="41">
         <v>30</v>
@@ -5339,7 +5339,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="49" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D21" s="41">
         <v>20</v>
@@ -5369,13 +5369,13 @@
         <v>22</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22" s="41">
         <v>42</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F22" s="43">
         <v>23</v>
@@ -5399,7 +5399,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D23" s="41">
         <v>42</v>
@@ -5429,7 +5429,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="50" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D24" s="41">
         <v>28</v>
@@ -5438,7 +5438,7 @@
         <v>23</v>
       </c>
       <c r="F24" s="43" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G24" s="43"/>
       <c r="H24" s="44"/>
@@ -5459,7 +5459,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="50" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D25" s="41">
         <v>42</v>
@@ -5468,7 +5468,7 @@
         <v>24</v>
       </c>
       <c r="F25" s="43" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G25" s="43"/>
       <c r="H25" s="44"/>
@@ -5489,13 +5489,13 @@
         <v>26</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D26" s="41">
         <v>30</v>
       </c>
       <c r="E26" s="43" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F26" s="43">
         <v>27</v>
@@ -5519,7 +5519,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D27" s="41">
         <v>30</v>
@@ -5549,7 +5549,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D28" s="41">
         <v>45</v>
@@ -5579,7 +5579,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D29" s="41">
         <v>50</v>
@@ -5609,13 +5609,13 @@
         <v>30</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D30" s="41">
         <v>60</v>
       </c>
       <c r="E30" s="43" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F30" s="43">
         <v>31</v>
@@ -5639,16 +5639,16 @@
         <v>31</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D31" s="41">
         <v>70</v>
       </c>
       <c r="E31" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="F31" s="43" t="s">
         <v>250</v>
-      </c>
-      <c r="F31" s="43" t="s">
-        <v>251</v>
       </c>
       <c r="G31" s="43"/>
       <c r="H31" s="44"/>
@@ -5669,16 +5669,16 @@
         <v>32</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D32" s="41">
         <v>50</v>
       </c>
       <c r="E32" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="F32" s="43" t="s">
         <v>252</v>
-      </c>
-      <c r="F32" s="43" t="s">
-        <v>253</v>
       </c>
       <c r="G32" s="43"/>
       <c r="H32" s="44"/>
@@ -5699,13 +5699,13 @@
         <v>33</v>
       </c>
       <c r="C33" s="52" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D33" s="41">
         <v>15</v>
       </c>
       <c r="E33" s="43" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F33" s="43">
         <v>34</v>
@@ -5737,13 +5737,13 @@
         <v>34</v>
       </c>
       <c r="C34" s="52" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D34" s="41">
         <v>15</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F34" s="43">
         <v>35</v>
@@ -5775,7 +5775,7 @@
         <v>35</v>
       </c>
       <c r="C35" s="52" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D35" s="41">
         <v>10</v>
@@ -5809,13 +5809,13 @@
         <v>36</v>
       </c>
       <c r="C36" s="52" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D36" s="41">
         <v>10</v>
       </c>
       <c r="E36" s="43" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F36" s="43">
         <v>37</v>
@@ -5845,7 +5845,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="52" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D37" s="41">
         <v>10</v>
@@ -5883,13 +5883,13 @@
         <v>38</v>
       </c>
       <c r="C38" s="53" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D38" s="41">
         <v>20</v>
       </c>
       <c r="E38" s="43" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F38" s="43">
         <v>39</v>
@@ -5925,7 +5925,7 @@
         <v>39</v>
       </c>
       <c r="C39" s="53" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D39" s="41">
         <v>30</v>
@@ -5957,7 +5957,7 @@
         <v>40</v>
       </c>
       <c r="C40" s="53" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D40" s="41">
         <v>0</v>
@@ -6951,27 +6951,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="27" t="s">
         <v>116</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>117</v>
       </c>
       <c r="D2" s="27">
         <v>3</v>
@@ -6979,13 +6979,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" s="27">
         <v>5</v>
@@ -6993,13 +6993,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D4" s="27">
         <v>2</v>
@@ -7007,13 +7007,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" s="27">
         <v>4</v>
@@ -7021,13 +7021,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" s="27">
         <v>1</v>
@@ -7035,13 +7035,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D7" s="27">
         <v>1</v>
@@ -7049,13 +7049,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D8" s="27">
         <v>1</v>
@@ -7063,13 +7063,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D9" s="27">
         <v>2</v>
@@ -7078,13 +7078,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D10" s="27">
         <v>1</v>
@@ -7092,13 +7092,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" s="27">
         <v>2</v>
@@ -7106,13 +7106,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12" s="27">
         <v>1</v>
@@ -7120,13 +7120,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D13" s="27">
         <v>2</v>

</xml_diff>